<commit_message>
Uploaded final set of supplementary for Chapter 4
</commit_message>
<xml_diff>
--- a/Chapter_04/Chapter_4_Table_S4.11.xlsx
+++ b/Chapter_04/Chapter_4_Table_S4.11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crtuser\OneDrive - National University of Ireland, Galway\Desktop\Dropbox\@John O'Grady\@Thesis\Supplementary\Chapter_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C9929B8-A82A-4F55-ADFE-66FE203C74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E50C8B70-B738-4BB6-868E-9AA97C919FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49170" yWindow="-1830" windowWidth="29040" windowHeight="15720" xr2:uid="{D73AC5C3-68BC-42E6-9C49-2009A566E965}"/>
+    <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{0ED7296C-EF11-40AA-867E-4E8FE970A8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter_4_Table_S4.11" sheetId="1" r:id="rId1"/>
@@ -83,43 +83,43 @@
     <t>SATB1</t>
   </si>
   <si>
-    <t>Pass 1</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1_LZTS3</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1_LZTS3_TTI2</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1_LZTS3_TTI2_SGMS1</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1_LZTS3_TTI2_SGMS1_UBASH3A</t>
-  </si>
-  <si>
-    <t>SATB1_ALAS1_NR4A2_MTM1_ELF2_ZNF75D_DCAF5_ASAH1_LZTS3_TTI2_SGMS1_UBASH3A_AKAP8</t>
+    <t>13-gene set</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3, MYB</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3, MYB, BCDIN3D</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3, MYB, BCDIN3D, TEX2</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3, MYB, BCDIN3D, TEX2, MAD2L2</t>
+  </si>
+  <si>
+    <t>SATB1, ALAS1, NR4A2, SMG8, ELP2, DCAF5, ZNF75D, PRICKLE3, MYB, BCDIN3D, TEX2, MAD2L2, KATNBL1</t>
   </si>
 </sst>
 </file>
@@ -221,18 +221,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B6D1FDC-AB28-4DA8-A485-78EABB3C5766}" name="Table11" displayName="Table11" ref="A2:I15" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68BCC6E0-5DE8-4E93-8052-01E763F42A22}" name="Table11" displayName="Table11" ref="A2:I15" totalsRowShown="0">
   <autoFilter ref="A2:I15" xr:uid="{D38A2450-C541-448E-9420-4212BE1D4AA2}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{85C720A3-2BF1-456C-A545-EC28F15D3C20}" name="combination" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{52CEC942-E88D-4303-BA63-D89171E01561}" name="Fold1"/>
-    <tableColumn id="3" xr3:uid="{3310EB15-09D5-4620-9197-C67634C1605F}" name="Fold2"/>
-    <tableColumn id="4" xr3:uid="{02C7E07B-86C6-44A5-ADCA-BFE98143686F}" name="Fold3"/>
-    <tableColumn id="5" xr3:uid="{611BDD62-A79D-48E3-BB33-0D0C07BAFC45}" name="Fold4"/>
-    <tableColumn id="6" xr3:uid="{2780CB56-4F13-46D3-9D47-24E655C6AFD6}" name="Fold5"/>
-    <tableColumn id="7" xr3:uid="{CCE1752C-766B-4C67-9EA7-8DFEB15526B5}" name="Average"/>
-    <tableColumn id="8" xr3:uid="{44E987F2-0D7A-493E-8566-4F5C75FE99D2}" name="Iteration"/>
-    <tableColumn id="9" xr3:uid="{71F5F49E-B1E9-4F82-BCDC-6DF10541ECCA}" name="Group"/>
+    <tableColumn id="1" xr3:uid="{BA73A4B3-224A-4E19-B03C-D9989CB01C73}" name="combination" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{3BC2F5E5-979E-4AC9-B303-4211EF537890}" name="Fold1"/>
+    <tableColumn id="3" xr3:uid="{8DD967FF-A714-4385-A1FB-2A91BD6C1879}" name="Fold2"/>
+    <tableColumn id="4" xr3:uid="{EBC28608-6DCA-4C9D-BB40-6B8EDCED56D7}" name="Fold3"/>
+    <tableColumn id="5" xr3:uid="{E910CD02-B2DD-4500-8475-C0B8DF3F5DDC}" name="Fold4"/>
+    <tableColumn id="6" xr3:uid="{8A98D36A-6119-42A7-87BE-A62504CB2466}" name="Fold5"/>
+    <tableColumn id="7" xr3:uid="{4432E599-9290-4B1B-A66F-B1E2F9149C26}" name="Average"/>
+    <tableColumn id="8" xr3:uid="{65CAD409-282E-4448-8C57-57A2E1F1E0ED}" name="Iteration"/>
+    <tableColumn id="9" xr3:uid="{1E6DDB97-A405-4897-A9D6-F8E3F03BDEE4}" name="Group"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -554,7 +554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE91CB4B-E95C-4B3C-92EE-D490733210CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCC1944-20BE-47B5-96F7-C890A3BCC37E}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K15"/>
   <sheetViews>
@@ -564,9 +564,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -584,7 +585,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -613,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -624,7 +625,7 @@
         <v>0.93188854489164097</v>
       </c>
       <c r="D3">
-        <v>0.60546875</v>
+        <v>0.61328125</v>
       </c>
       <c r="E3">
         <v>0.77083333333333304</v>
@@ -633,7 +634,7 @@
         <v>0.81410256410256399</v>
       </c>
       <c r="G3">
-        <v>0.79452666567639196</v>
+        <v>0.79608916567639199</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -642,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -671,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -700,27 +701,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.969387755102041</v>
+        <v>0.96598639455782298</v>
       </c>
       <c r="C6">
-        <v>0.96594427244582004</v>
+        <v>0.97213622291021695</v>
       </c>
       <c r="D6">
-        <v>0.9375</v>
+        <v>0.91015625</v>
       </c>
       <c r="E6">
-        <v>0.95416666666666705</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F6">
-        <v>0.96153846153846201</v>
+        <v>0.94230769230769196</v>
       </c>
       <c r="G6">
-        <v>0.95770743115059798</v>
+        <v>0.95311731195514604</v>
       </c>
       <c r="H6">
         <v>4</v>
@@ -729,27 +730,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.97619047619047605</v>
+        <v>0.97959183673469397</v>
       </c>
       <c r="C7">
-        <v>0.97832817337461297</v>
+        <v>0.98142414860681104</v>
       </c>
       <c r="D7">
-        <v>0.9609375</v>
+        <v>0.9453125</v>
       </c>
       <c r="E7">
         <v>0.95416666666666705</v>
       </c>
       <c r="F7">
-        <v>0.95512820512820495</v>
+        <v>0.93589743589743601</v>
       </c>
       <c r="G7">
-        <v>0.96495020427199196</v>
+        <v>0.95927851758112104</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -758,27 +759,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.969387755102041</v>
+        <v>0.97959183673469397</v>
       </c>
       <c r="C8">
-        <v>0.96284829721362197</v>
+        <v>0.98142414860681104</v>
       </c>
       <c r="D8">
-        <v>0.97265625</v>
+        <v>0.94921875</v>
       </c>
       <c r="E8">
-        <v>0.96250000000000002</v>
+        <v>0.98333333333333295</v>
       </c>
       <c r="F8">
-        <v>0.96794871794871795</v>
+        <v>0.96153846153846201</v>
       </c>
       <c r="G8">
-        <v>0.96706820405287597</v>
+        <v>0.97102130604266002</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -787,27 +788,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.97959183673469397</v>
+        <v>0.98299319727891199</v>
       </c>
       <c r="C9">
-        <v>0.984520123839009</v>
+        <v>0.98761609907120695</v>
       </c>
       <c r="D9">
-        <v>0.96484375</v>
+        <v>0.95703125</v>
       </c>
       <c r="E9">
-        <v>0.96250000000000002</v>
+        <v>0.97916666666666696</v>
       </c>
       <c r="F9">
-        <v>0.98076923076923095</v>
+        <v>0.96153846153846201</v>
       </c>
       <c r="G9">
-        <v>0.97444498826858705</v>
+        <v>0.97366913491104901</v>
       </c>
       <c r="H9">
         <v>7</v>
@@ -816,27 +817,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0.97959183673469397</v>
+        <v>0.98639455782312901</v>
       </c>
       <c r="C10">
-        <v>0.98761609907120695</v>
+        <v>0.97523219814241502</v>
       </c>
       <c r="D10">
-        <v>0.984375</v>
+        <v>0.96484375</v>
       </c>
       <c r="E10">
-        <v>0.97083333333333299</v>
+        <v>0.97916666666666696</v>
       </c>
       <c r="F10">
-        <v>0.987179487179487</v>
+        <v>0.99358974358974395</v>
       </c>
       <c r="G10">
-        <v>0.98191915126374396</v>
+        <v>0.97984538324439097</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -845,27 +846,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11">
-        <v>0.97619047619047605</v>
+        <v>0.98299319727891199</v>
       </c>
       <c r="C11">
-        <v>0.98142414860681104</v>
+        <v>0.98761609907120695</v>
       </c>
       <c r="D11">
-        <v>0.96484375</v>
+        <v>0.98828125</v>
       </c>
       <c r="E11">
-        <v>0.99166666666666703</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0.98076923076923095</v>
       </c>
       <c r="G11">
-        <v>0.98282500829279096</v>
+        <v>0.98543195542386997</v>
       </c>
       <c r="H11">
         <v>9</v>
@@ -874,7 +875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -882,10 +883,10 @@
         <v>0.98299319727891199</v>
       </c>
       <c r="C12">
-        <v>0.98761609907120695</v>
+        <v>0.97832817337461297</v>
       </c>
       <c r="D12">
-        <v>0.984375</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0.99166666666666703</v>
@@ -894,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.98933019260335697</v>
+        <v>0.99059760746403802</v>
       </c>
       <c r="H12">
         <v>10</v>
@@ -903,27 +904,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B13">
-        <v>0.98639455782312901</v>
+        <v>0.98979591836734704</v>
       </c>
       <c r="C13">
+        <v>0.99380804953560398</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>0.984375</v>
-      </c>
       <c r="E13">
-        <v>0.98750000000000004</v>
+        <v>0.98333333333333295</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.99165391156462601</v>
+        <v>0.99338746024725699</v>
       </c>
       <c r="H13">
         <v>11</v>
@@ -932,27 +933,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B14">
-        <v>0.99319727891156495</v>
+        <v>0.98979591836734704</v>
       </c>
       <c r="C14">
-        <v>0.99380804953560398</v>
+        <v>0.98761609907120695</v>
       </c>
       <c r="D14">
-        <v>0.98046875</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0.99166666666666703</v>
+        <v>0.99583333333333302</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0.99182814902276695</v>
+        <v>0.99464907015437798</v>
       </c>
       <c r="H14">
         <v>12</v>
@@ -961,18 +962,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B15">
-        <v>0.99319727891156495</v>
+        <v>0.98979591836734704</v>
       </c>
       <c r="C15">
-        <v>0.98761609907120695</v>
+        <v>0.99380804953560398</v>
       </c>
       <c r="D15">
-        <v>0.98828125</v>
+        <v>0.99609375</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -981,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>0.99381892559655405</v>
+        <v>0.99593954358059</v>
       </c>
       <c r="H15">
         <v>13</v>

</xml_diff>